<commit_message>
Arrays are shit. but they are done
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="493">
   <si>
     <t>Topic:</t>
   </si>
@@ -1501,6 +1501,9 @@
   </si>
   <si>
     <t>5,4</t>
+  </si>
+  <si>
+    <t>07-05-2021 mark</t>
   </si>
 </sst>
 </file>
@@ -1975,7 +1978,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2258,8 +2261,8 @@
       <c r="B28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>3</v>
+      <c r="C28" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21">
@@ -2269,8 +2272,8 @@
       <c r="B29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>3</v>
+      <c r="C29" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21">
@@ -2280,8 +2283,8 @@
       <c r="B30" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>3</v>
+      <c r="C30" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21">
@@ -2291,8 +2294,8 @@
       <c r="B31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>3</v>
+      <c r="C31" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21">
@@ -2302,8 +2305,8 @@
       <c r="B32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>3</v>
+      <c r="C32" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="21">
@@ -2313,8 +2316,8 @@
       <c r="B33" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>3</v>
+      <c r="C33" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="21">
@@ -2324,8 +2327,8 @@
       <c r="B34" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>3</v>
+      <c r="C34" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21">
@@ -2335,8 +2338,8 @@
       <c r="B35" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>3</v>
+      <c r="C35" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="21">
@@ -2346,8 +2349,8 @@
       <c r="B36" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>3</v>
+      <c r="C36" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21">
@@ -2492,7 +2495,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>3</v>
+        <v>492</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Matrix plus 2 stock
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="494">
   <si>
     <t>Topic:</t>
   </si>
@@ -1504,6 +1504,9 @@
   </si>
   <si>
     <t>07-05-2021 mark</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1975,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C481"/>
+  <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2360,8 +2363,8 @@
       <c r="B37" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>3</v>
+      <c r="C37" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="21">
@@ -2371,8 +2374,8 @@
       <c r="B38" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>3</v>
+      <c r="C38" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="21">
@@ -2382,8 +2385,8 @@
       <c r="B39" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>3</v>
+      <c r="C39" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21">
@@ -2393,8 +2396,8 @@
       <c r="B40" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>3</v>
+      <c r="C40" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="21">
@@ -2404,8 +2407,8 @@
       <c r="B41" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>3</v>
+      <c r="C41" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21">
@@ -2476,7 +2479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="21">
+    <row r="49" spans="1:5" ht="21">
       <c r="A49" s="8" t="s">
         <v>41</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21">
+    <row r="50" spans="1:5" ht="21">
       <c r="A50" s="8" t="s">
         <v>41</v>
       </c>
@@ -2498,7 +2501,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="21">
+    <row r="51" spans="1:5" ht="21">
       <c r="A51" s="8" t="s">
         <v>41</v>
       </c>
@@ -2509,7 +2512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21">
+    <row r="52" spans="1:5" ht="21">
       <c r="A52" s="8" t="s">
         <v>41</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="21">
+    <row r="53" spans="1:5" ht="21">
       <c r="A53" s="8" t="s">
         <v>41</v>
       </c>
@@ -2531,12 +2534,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="21">
+    <row r="55" spans="1:5" ht="21">
       <c r="A55" s="5"/>
       <c r="B55" s="7"/>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:3" ht="21">
+    <row r="56" spans="1:5" ht="21">
       <c r="A56" s="5" t="s">
         <v>52</v>
       </c>
@@ -2547,7 +2550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="21">
+    <row r="57" spans="1:5" ht="21">
       <c r="A57" s="5" t="s">
         <v>52</v>
       </c>
@@ -2558,7 +2561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="21">
+    <row r="58" spans="1:5" ht="21">
       <c r="A58" s="5" t="s">
         <v>52</v>
       </c>
@@ -2569,7 +2572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="21">
+    <row r="59" spans="1:5" ht="21">
       <c r="A59" s="5" t="s">
         <v>52</v>
       </c>
@@ -2580,7 +2583,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="21">
+    <row r="60" spans="1:5" ht="21">
       <c r="A60" s="5" t="s">
         <v>52</v>
       </c>
@@ -2591,7 +2594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="21">
+    <row r="61" spans="1:5" ht="21">
       <c r="A61" s="5" t="s">
         <v>52</v>
       </c>
@@ -2602,7 +2605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="21">
+    <row r="62" spans="1:5" ht="21">
       <c r="A62" s="5" t="s">
         <v>52</v>
       </c>
@@ -2613,7 +2616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="21">
+    <row r="63" spans="1:5" ht="21">
       <c r="A63" s="5" t="s">
         <v>52</v>
       </c>
@@ -2624,7 +2627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="21">
+    <row r="64" spans="1:5" ht="21">
       <c r="A64" s="5" t="s">
         <v>52</v>
       </c>
@@ -2633,6 +2636,9 @@
       </c>
       <c r="C64" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">

</xml_diff>

<commit_message>
1 1 approach started
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1504,10 +1503,10 @@
     <t>5,4</t>
   </si>
   <si>
-    <t>07-05-2021 mark</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>not understood</t>
   </si>
 </sst>
 </file>
@@ -1981,8 +1980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2432,8 +2431,8 @@
       <c r="B44" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>3</v>
+      <c r="C44" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">
@@ -2443,8 +2442,8 @@
       <c r="B45" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>3</v>
+      <c r="C45" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="21">
@@ -2454,8 +2453,8 @@
       <c r="B46" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>3</v>
+      <c r="C46" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="21">
@@ -2465,8 +2464,8 @@
       <c r="B47" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>3</v>
+      <c r="C47" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="21">
@@ -2476,8 +2475,8 @@
       <c r="B48" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>3</v>
+      <c r="C48" s="11" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="21">
@@ -2487,8 +2486,8 @@
       <c r="B49" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>3</v>
+      <c r="C49" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="21">
@@ -2498,8 +2497,8 @@
       <c r="B50" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>492</v>
+      <c r="C50" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="21">
@@ -2547,8 +2546,8 @@
       <c r="B56" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>3</v>
+      <c r="C56" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="21">
@@ -2639,7 +2638,7 @@
         <v>3</v>
       </c>
       <c r="E64" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">
@@ -3028,8 +3027,8 @@
       <c r="B101" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C101" s="4" t="s">
-        <v>3</v>
+      <c r="C101" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="21">
@@ -3428,8 +3427,8 @@
       <c r="B139" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C139" s="4" t="s">
-        <v>3</v>
+      <c r="C139" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21">
@@ -7138,369 +7137,369 @@
     <hyperlink ref="B96" r:id="rId81"/>
     <hyperlink ref="B97" r:id="rId82"/>
     <hyperlink ref="B98" r:id="rId83"/>
-    <hyperlink ref="B101" r:id="rId84"/>
-    <hyperlink ref="B102" r:id="rId85"/>
-    <hyperlink ref="B103" r:id="rId86"/>
-    <hyperlink ref="B104" r:id="rId87"/>
-    <hyperlink ref="B106" r:id="rId88" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
-    <hyperlink ref="B107" r:id="rId89"/>
-    <hyperlink ref="B108" r:id="rId90"/>
-    <hyperlink ref="B109" r:id="rId91"/>
-    <hyperlink ref="B110" r:id="rId92"/>
-    <hyperlink ref="B111" r:id="rId93"/>
-    <hyperlink ref="B113" r:id="rId94"/>
-    <hyperlink ref="B114" r:id="rId95"/>
-    <hyperlink ref="B115" r:id="rId96"/>
-    <hyperlink ref="B116" r:id="rId97"/>
-    <hyperlink ref="B117" r:id="rId98"/>
-    <hyperlink ref="B118" r:id="rId99"/>
-    <hyperlink ref="B119" r:id="rId100"/>
-    <hyperlink ref="B120" r:id="rId101"/>
-    <hyperlink ref="B121" r:id="rId102"/>
-    <hyperlink ref="B122" r:id="rId103"/>
-    <hyperlink ref="B123" r:id="rId104"/>
-    <hyperlink ref="B124" r:id="rId105"/>
-    <hyperlink ref="B125" r:id="rId106"/>
-    <hyperlink ref="B126" r:id="rId107"/>
-    <hyperlink ref="B127" r:id="rId108"/>
-    <hyperlink ref="B128" r:id="rId109"/>
-    <hyperlink ref="B129" r:id="rId110"/>
-    <hyperlink ref="B130" r:id="rId111"/>
-    <hyperlink ref="B131" r:id="rId112"/>
-    <hyperlink ref="B132" r:id="rId113"/>
-    <hyperlink ref="B133" r:id="rId114"/>
-    <hyperlink ref="B134" r:id="rId115"/>
-    <hyperlink ref="B135" r:id="rId116"/>
-    <hyperlink ref="B136" r:id="rId117"/>
-    <hyperlink ref="B105" r:id="rId118"/>
-    <hyperlink ref="B112" r:id="rId119"/>
-    <hyperlink ref="B139" r:id="rId120"/>
-    <hyperlink ref="B140" r:id="rId121"/>
-    <hyperlink ref="B141" r:id="rId122"/>
-    <hyperlink ref="B142" r:id="rId123"/>
-    <hyperlink ref="B143" r:id="rId124"/>
-    <hyperlink ref="B144" r:id="rId125"/>
-    <hyperlink ref="B145" r:id="rId126"/>
-    <hyperlink ref="B146" r:id="rId127"/>
-    <hyperlink ref="B147" r:id="rId128"/>
-    <hyperlink ref="B148" r:id="rId129"/>
-    <hyperlink ref="B149" r:id="rId130"/>
-    <hyperlink ref="B150" r:id="rId131"/>
-    <hyperlink ref="B151" r:id="rId132"/>
-    <hyperlink ref="B152" r:id="rId133"/>
-    <hyperlink ref="B153" r:id="rId134"/>
-    <hyperlink ref="B154" r:id="rId135"/>
-    <hyperlink ref="B155" r:id="rId136"/>
-    <hyperlink ref="B156" r:id="rId137"/>
-    <hyperlink ref="B157" r:id="rId138"/>
-    <hyperlink ref="B158" r:id="rId139"/>
-    <hyperlink ref="B159" r:id="rId140"/>
-    <hyperlink ref="B160" r:id="rId141"/>
-    <hyperlink ref="B161" r:id="rId142"/>
-    <hyperlink ref="B162" r:id="rId143"/>
-    <hyperlink ref="B163" r:id="rId144"/>
-    <hyperlink ref="B166" r:id="rId145"/>
-    <hyperlink ref="B167" r:id="rId146"/>
-    <hyperlink ref="B168" r:id="rId147"/>
-    <hyperlink ref="B169" r:id="rId148"/>
-    <hyperlink ref="B170" r:id="rId149"/>
-    <hyperlink ref="B171" r:id="rId150"/>
-    <hyperlink ref="B172" r:id="rId151"/>
-    <hyperlink ref="B173" r:id="rId152"/>
-    <hyperlink ref="B174" r:id="rId153"/>
-    <hyperlink ref="B177" r:id="rId154"/>
-    <hyperlink ref="B178" r:id="rId155"/>
-    <hyperlink ref="B179" r:id="rId156"/>
-    <hyperlink ref="B180" r:id="rId157"/>
-    <hyperlink ref="B181" r:id="rId158"/>
-    <hyperlink ref="B182" r:id="rId159"/>
-    <hyperlink ref="B183" r:id="rId160"/>
-    <hyperlink ref="B184" r:id="rId161"/>
-    <hyperlink ref="B185" r:id="rId162"/>
-    <hyperlink ref="B186" r:id="rId163"/>
-    <hyperlink ref="B187" r:id="rId164"/>
-    <hyperlink ref="B188" r:id="rId165"/>
-    <hyperlink ref="B189" r:id="rId166"/>
-    <hyperlink ref="B190" r:id="rId167"/>
-    <hyperlink ref="B191" r:id="rId168"/>
-    <hyperlink ref="B192" r:id="rId169"/>
-    <hyperlink ref="B193" r:id="rId170"/>
-    <hyperlink ref="B194" r:id="rId171"/>
-    <hyperlink ref="B195" r:id="rId172"/>
-    <hyperlink ref="B196" r:id="rId173"/>
-    <hyperlink ref="B197" r:id="rId174" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
-    <hyperlink ref="B198" r:id="rId175"/>
-    <hyperlink ref="B199" r:id="rId176"/>
-    <hyperlink ref="B200" r:id="rId177"/>
-    <hyperlink ref="B201" r:id="rId178"/>
-    <hyperlink ref="B202" r:id="rId179"/>
-    <hyperlink ref="B203" r:id="rId180" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
-    <hyperlink ref="B204" r:id="rId181"/>
-    <hyperlink ref="B205" r:id="rId182"/>
-    <hyperlink ref="B206" r:id="rId183"/>
-    <hyperlink ref="B207" r:id="rId184"/>
-    <hyperlink ref="B208" r:id="rId185"/>
-    <hyperlink ref="B209" r:id="rId186"/>
-    <hyperlink ref="B210" r:id="rId187"/>
-    <hyperlink ref="B211" r:id="rId188"/>
-    <hyperlink ref="B214" r:id="rId189"/>
-    <hyperlink ref="B215" r:id="rId190"/>
-    <hyperlink ref="B216" r:id="rId191"/>
-    <hyperlink ref="B217" r:id="rId192"/>
-    <hyperlink ref="B218" r:id="rId193"/>
-    <hyperlink ref="B219" r:id="rId194"/>
-    <hyperlink ref="B220" r:id="rId195"/>
-    <hyperlink ref="B221" r:id="rId196"/>
-    <hyperlink ref="B222" r:id="rId197"/>
-    <hyperlink ref="B223" r:id="rId198"/>
-    <hyperlink ref="B224" r:id="rId199"/>
-    <hyperlink ref="B225" r:id="rId200"/>
-    <hyperlink ref="B226" r:id="rId201"/>
-    <hyperlink ref="B227" r:id="rId202"/>
-    <hyperlink ref="B228" r:id="rId203"/>
-    <hyperlink ref="B229" r:id="rId204"/>
-    <hyperlink ref="B230" r:id="rId205"/>
-    <hyperlink ref="B231" r:id="rId206"/>
-    <hyperlink ref="B232" r:id="rId207"/>
-    <hyperlink ref="B233" r:id="rId208"/>
-    <hyperlink ref="B234" r:id="rId209"/>
-    <hyperlink ref="B235" r:id="rId210"/>
-    <hyperlink ref="B238" r:id="rId211"/>
-    <hyperlink ref="B239" r:id="rId212"/>
-    <hyperlink ref="B240" r:id="rId213"/>
-    <hyperlink ref="B241" r:id="rId214"/>
-    <hyperlink ref="B242" r:id="rId215"/>
-    <hyperlink ref="B243" r:id="rId216"/>
-    <hyperlink ref="B244" r:id="rId217"/>
-    <hyperlink ref="B245" r:id="rId218"/>
-    <hyperlink ref="B246" r:id="rId219"/>
-    <hyperlink ref="B247" r:id="rId220"/>
-    <hyperlink ref="B248" r:id="rId221"/>
-    <hyperlink ref="B249" r:id="rId222"/>
-    <hyperlink ref="B250" r:id="rId223"/>
-    <hyperlink ref="B251" r:id="rId224"/>
-    <hyperlink ref="B252" r:id="rId225"/>
-    <hyperlink ref="B253" r:id="rId226"/>
-    <hyperlink ref="B254" r:id="rId227"/>
-    <hyperlink ref="B255" r:id="rId228"/>
-    <hyperlink ref="B256" r:id="rId229"/>
-    <hyperlink ref="B257" r:id="rId230" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="B258" r:id="rId231"/>
-    <hyperlink ref="B259" r:id="rId232"/>
-    <hyperlink ref="B260" r:id="rId233"/>
-    <hyperlink ref="B261" r:id="rId234"/>
-    <hyperlink ref="B262" r:id="rId235"/>
-    <hyperlink ref="B263" r:id="rId236"/>
-    <hyperlink ref="B264" r:id="rId237"/>
-    <hyperlink ref="B265" r:id="rId238"/>
-    <hyperlink ref="B266" r:id="rId239"/>
-    <hyperlink ref="B267" r:id="rId240"/>
-    <hyperlink ref="B268" r:id="rId241"/>
-    <hyperlink ref="B269" r:id="rId242"/>
-    <hyperlink ref="B270" r:id="rId243"/>
-    <hyperlink ref="B271" r:id="rId244"/>
-    <hyperlink ref="B272" r:id="rId245"/>
-    <hyperlink ref="B275" r:id="rId246"/>
-    <hyperlink ref="B276" r:id="rId247"/>
-    <hyperlink ref="B277" r:id="rId248"/>
-    <hyperlink ref="B278" r:id="rId249"/>
-    <hyperlink ref="B279" r:id="rId250"/>
-    <hyperlink ref="B280" r:id="rId251"/>
-    <hyperlink ref="B281" r:id="rId252"/>
-    <hyperlink ref="B282" r:id="rId253"/>
-    <hyperlink ref="B283" r:id="rId254"/>
-    <hyperlink ref="B284" r:id="rId255"/>
-    <hyperlink ref="B285" r:id="rId256"/>
-    <hyperlink ref="B286" r:id="rId257"/>
-    <hyperlink ref="B287" r:id="rId258"/>
-    <hyperlink ref="B288" r:id="rId259"/>
-    <hyperlink ref="B289" r:id="rId260"/>
-    <hyperlink ref="B290" r:id="rId261"/>
-    <hyperlink ref="B291" r:id="rId262"/>
-    <hyperlink ref="B292" r:id="rId263"/>
-    <hyperlink ref="B293" r:id="rId264"/>
-    <hyperlink ref="B296" r:id="rId265"/>
-    <hyperlink ref="B297" r:id="rId266"/>
-    <hyperlink ref="B298" r:id="rId267"/>
-    <hyperlink ref="B299" r:id="rId268"/>
-    <hyperlink ref="B300" r:id="rId269"/>
-    <hyperlink ref="B301" r:id="rId270"/>
-    <hyperlink ref="B302" r:id="rId271"/>
-    <hyperlink ref="B303" r:id="rId272"/>
-    <hyperlink ref="B304" r:id="rId273"/>
-    <hyperlink ref="B305" r:id="rId274"/>
-    <hyperlink ref="B306" r:id="rId275" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
-    <hyperlink ref="B307" r:id="rId276"/>
-    <hyperlink ref="B308" r:id="rId277"/>
-    <hyperlink ref="B309" r:id="rId278"/>
-    <hyperlink ref="B310" r:id="rId279"/>
-    <hyperlink ref="B311" r:id="rId280"/>
-    <hyperlink ref="B312" r:id="rId281"/>
-    <hyperlink ref="B313" r:id="rId282"/>
-    <hyperlink ref="B314" r:id="rId283"/>
-    <hyperlink ref="B315" r:id="rId284"/>
-    <hyperlink ref="B316" r:id="rId285"/>
-    <hyperlink ref="B317" r:id="rId286"/>
-    <hyperlink ref="B318" r:id="rId287"/>
-    <hyperlink ref="B319" r:id="rId288"/>
-    <hyperlink ref="B320" r:id="rId289"/>
-    <hyperlink ref="B321" r:id="rId290"/>
-    <hyperlink ref="B322" r:id="rId291"/>
-    <hyperlink ref="B323" r:id="rId292"/>
-    <hyperlink ref="B324" r:id="rId293"/>
-    <hyperlink ref="B325" r:id="rId294"/>
-    <hyperlink ref="B326" r:id="rId295"/>
-    <hyperlink ref="B327" r:id="rId296"/>
-    <hyperlink ref="B328" r:id="rId297"/>
-    <hyperlink ref="B329" r:id="rId298"/>
-    <hyperlink ref="B330" r:id="rId299"/>
-    <hyperlink ref="B331" r:id="rId300"/>
-    <hyperlink ref="B332" r:id="rId301"/>
-    <hyperlink ref="B333" r:id="rId302"/>
-    <hyperlink ref="B336" r:id="rId303"/>
-    <hyperlink ref="B337" r:id="rId304"/>
-    <hyperlink ref="B338" r:id="rId305"/>
-    <hyperlink ref="B339" r:id="rId306"/>
-    <hyperlink ref="B340" r:id="rId307"/>
-    <hyperlink ref="B341" r:id="rId308"/>
-    <hyperlink ref="B342" r:id="rId309"/>
-    <hyperlink ref="B343" r:id="rId310"/>
-    <hyperlink ref="B344" r:id="rId311"/>
-    <hyperlink ref="B345" r:id="rId312"/>
-    <hyperlink ref="B346" r:id="rId313"/>
-    <hyperlink ref="B347" r:id="rId314"/>
-    <hyperlink ref="B348" r:id="rId315"/>
-    <hyperlink ref="B349" r:id="rId316"/>
-    <hyperlink ref="B350" r:id="rId317"/>
-    <hyperlink ref="B351" r:id="rId318"/>
-    <hyperlink ref="B352" r:id="rId319"/>
-    <hyperlink ref="B353" r:id="rId320"/>
-    <hyperlink ref="B357" r:id="rId321"/>
-    <hyperlink ref="B358" r:id="rId322"/>
-    <hyperlink ref="B359" r:id="rId323"/>
-    <hyperlink ref="B360" r:id="rId324"/>
-    <hyperlink ref="B361" r:id="rId325"/>
-    <hyperlink ref="B362" r:id="rId326"/>
-    <hyperlink ref="B363" r:id="rId327"/>
-    <hyperlink ref="B364" r:id="rId328"/>
-    <hyperlink ref="B365" r:id="rId329"/>
-    <hyperlink ref="B366" r:id="rId330"/>
-    <hyperlink ref="B367" r:id="rId331"/>
-    <hyperlink ref="B368" r:id="rId332"/>
-    <hyperlink ref="B369" r:id="rId333"/>
-    <hyperlink ref="B370" r:id="rId334"/>
-    <hyperlink ref="B371" r:id="rId335"/>
-    <hyperlink ref="B372" r:id="rId336"/>
-    <hyperlink ref="B373" r:id="rId337"/>
-    <hyperlink ref="B374" r:id="rId338"/>
-    <hyperlink ref="B375" r:id="rId339"/>
-    <hyperlink ref="B376" r:id="rId340"/>
-    <hyperlink ref="B377" r:id="rId341"/>
-    <hyperlink ref="B378" r:id="rId342"/>
-    <hyperlink ref="B379" r:id="rId343" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="B380" r:id="rId344"/>
-    <hyperlink ref="B381" r:id="rId345"/>
-    <hyperlink ref="B382" r:id="rId346"/>
-    <hyperlink ref="B383" r:id="rId347"/>
-    <hyperlink ref="B384" r:id="rId348"/>
-    <hyperlink ref="B385" r:id="rId349"/>
-    <hyperlink ref="B386" r:id="rId350"/>
-    <hyperlink ref="B387" r:id="rId351"/>
-    <hyperlink ref="B388" r:id="rId352"/>
-    <hyperlink ref="B389" r:id="rId353"/>
-    <hyperlink ref="B390" r:id="rId354"/>
-    <hyperlink ref="B391" r:id="rId355"/>
-    <hyperlink ref="B392" r:id="rId356"/>
-    <hyperlink ref="B393" r:id="rId357"/>
-    <hyperlink ref="B394" r:id="rId358"/>
-    <hyperlink ref="B396" r:id="rId359"/>
-    <hyperlink ref="B395" r:id="rId360"/>
-    <hyperlink ref="B397" r:id="rId361"/>
-    <hyperlink ref="B398" r:id="rId362"/>
-    <hyperlink ref="B399" r:id="rId363"/>
-    <hyperlink ref="B402" r:id="rId364"/>
-    <hyperlink ref="B403" r:id="rId365"/>
-    <hyperlink ref="B404" r:id="rId366"/>
-    <hyperlink ref="B405" r:id="rId367"/>
-    <hyperlink ref="B406" r:id="rId368"/>
-    <hyperlink ref="B407" r:id="rId369"/>
-    <hyperlink ref="B410" r:id="rId370"/>
-    <hyperlink ref="B411" r:id="rId371"/>
-    <hyperlink ref="B412" r:id="rId372"/>
-    <hyperlink ref="B413" r:id="rId373"/>
-    <hyperlink ref="B414" r:id="rId374"/>
-    <hyperlink ref="B415" r:id="rId375"/>
-    <hyperlink ref="B416" r:id="rId376"/>
-    <hyperlink ref="B417" r:id="rId377"/>
-    <hyperlink ref="B418" r:id="rId378"/>
-    <hyperlink ref="B419" r:id="rId379"/>
-    <hyperlink ref="B420" r:id="rId380"/>
-    <hyperlink ref="B421" r:id="rId381"/>
-    <hyperlink ref="B422" r:id="rId382"/>
-    <hyperlink ref="B423" r:id="rId383"/>
-    <hyperlink ref="B424" r:id="rId384"/>
-    <hyperlink ref="B425" r:id="rId385"/>
-    <hyperlink ref="B426" r:id="rId386"/>
-    <hyperlink ref="B427" r:id="rId387"/>
-    <hyperlink ref="B428" r:id="rId388"/>
-    <hyperlink ref="B429" r:id="rId389"/>
-    <hyperlink ref="B430" r:id="rId390"/>
-    <hyperlink ref="B431" r:id="rId391"/>
-    <hyperlink ref="B432" r:id="rId392"/>
-    <hyperlink ref="B433" r:id="rId393"/>
-    <hyperlink ref="B434" r:id="rId394"/>
-    <hyperlink ref="B435" r:id="rId395"/>
-    <hyperlink ref="B436" r:id="rId396"/>
-    <hyperlink ref="B437" r:id="rId397"/>
-    <hyperlink ref="B438" r:id="rId398"/>
-    <hyperlink ref="B439" r:id="rId399"/>
-    <hyperlink ref="B440" r:id="rId400"/>
-    <hyperlink ref="B441" r:id="rId401"/>
-    <hyperlink ref="B442" r:id="rId402"/>
-    <hyperlink ref="B443" r:id="rId403"/>
-    <hyperlink ref="B444" r:id="rId404"/>
-    <hyperlink ref="B445" r:id="rId405"/>
-    <hyperlink ref="B446" r:id="rId406"/>
-    <hyperlink ref="B447" r:id="rId407"/>
-    <hyperlink ref="B448" r:id="rId408"/>
-    <hyperlink ref="B449" r:id="rId409"/>
-    <hyperlink ref="B451" r:id="rId410"/>
-    <hyperlink ref="B450" r:id="rId411"/>
-    <hyperlink ref="B452" r:id="rId412"/>
-    <hyperlink ref="B453" r:id="rId413"/>
-    <hyperlink ref="B454" r:id="rId414"/>
-    <hyperlink ref="B455" r:id="rId415"/>
-    <hyperlink ref="B456" r:id="rId416"/>
-    <hyperlink ref="B457" r:id="rId417"/>
-    <hyperlink ref="B458" r:id="rId418"/>
-    <hyperlink ref="B459" r:id="rId419"/>
-    <hyperlink ref="B460" r:id="rId420"/>
-    <hyperlink ref="B461" r:id="rId421"/>
-    <hyperlink ref="B462" r:id="rId422"/>
-    <hyperlink ref="B469" r:id="rId423"/>
-    <hyperlink ref="B468" r:id="rId424"/>
-    <hyperlink ref="B467" r:id="rId425"/>
-    <hyperlink ref="B466" r:id="rId426"/>
-    <hyperlink ref="B465" r:id="rId427"/>
-    <hyperlink ref="B464" r:id="rId428"/>
-    <hyperlink ref="B463" r:id="rId429"/>
-    <hyperlink ref="B472" r:id="rId430"/>
-    <hyperlink ref="B473" r:id="rId431"/>
-    <hyperlink ref="B474" r:id="rId432"/>
-    <hyperlink ref="B475" r:id="rId433"/>
-    <hyperlink ref="B476" r:id="rId434"/>
-    <hyperlink ref="B477" r:id="rId435"/>
-    <hyperlink ref="B478" r:id="rId436"/>
-    <hyperlink ref="B481" r:id="rId437"/>
-    <hyperlink ref="B479" r:id="rId438"/>
-    <hyperlink ref="B480" r:id="rId439" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B356" r:id="rId440"/>
-    <hyperlink ref="B2" r:id="rId441"/>
-    <hyperlink ref="B16" r:id="rId442"/>
-    <hyperlink ref="B15" r:id="rId443"/>
-    <hyperlink ref="B14" r:id="rId444"/>
-    <hyperlink ref="B13" r:id="rId445"/>
-    <hyperlink ref="B26" r:id="rId446"/>
+    <hyperlink ref="B102" r:id="rId84"/>
+    <hyperlink ref="B103" r:id="rId85"/>
+    <hyperlink ref="B104" r:id="rId86"/>
+    <hyperlink ref="B106" r:id="rId87" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
+    <hyperlink ref="B107" r:id="rId88"/>
+    <hyperlink ref="B108" r:id="rId89"/>
+    <hyperlink ref="B109" r:id="rId90"/>
+    <hyperlink ref="B110" r:id="rId91"/>
+    <hyperlink ref="B111" r:id="rId92"/>
+    <hyperlink ref="B113" r:id="rId93"/>
+    <hyperlink ref="B114" r:id="rId94"/>
+    <hyperlink ref="B115" r:id="rId95"/>
+    <hyperlink ref="B116" r:id="rId96"/>
+    <hyperlink ref="B117" r:id="rId97"/>
+    <hyperlink ref="B118" r:id="rId98"/>
+    <hyperlink ref="B119" r:id="rId99"/>
+    <hyperlink ref="B120" r:id="rId100"/>
+    <hyperlink ref="B121" r:id="rId101"/>
+    <hyperlink ref="B122" r:id="rId102"/>
+    <hyperlink ref="B123" r:id="rId103"/>
+    <hyperlink ref="B124" r:id="rId104"/>
+    <hyperlink ref="B125" r:id="rId105"/>
+    <hyperlink ref="B126" r:id="rId106"/>
+    <hyperlink ref="B127" r:id="rId107"/>
+    <hyperlink ref="B128" r:id="rId108"/>
+    <hyperlink ref="B129" r:id="rId109"/>
+    <hyperlink ref="B130" r:id="rId110"/>
+    <hyperlink ref="B131" r:id="rId111"/>
+    <hyperlink ref="B132" r:id="rId112"/>
+    <hyperlink ref="B133" r:id="rId113"/>
+    <hyperlink ref="B134" r:id="rId114"/>
+    <hyperlink ref="B135" r:id="rId115"/>
+    <hyperlink ref="B136" r:id="rId116"/>
+    <hyperlink ref="B105" r:id="rId117"/>
+    <hyperlink ref="B112" r:id="rId118"/>
+    <hyperlink ref="B139" r:id="rId119"/>
+    <hyperlink ref="B140" r:id="rId120"/>
+    <hyperlink ref="B141" r:id="rId121"/>
+    <hyperlink ref="B142" r:id="rId122"/>
+    <hyperlink ref="B143" r:id="rId123"/>
+    <hyperlink ref="B144" r:id="rId124"/>
+    <hyperlink ref="B145" r:id="rId125"/>
+    <hyperlink ref="B146" r:id="rId126"/>
+    <hyperlink ref="B147" r:id="rId127"/>
+    <hyperlink ref="B148" r:id="rId128"/>
+    <hyperlink ref="B149" r:id="rId129"/>
+    <hyperlink ref="B150" r:id="rId130"/>
+    <hyperlink ref="B151" r:id="rId131"/>
+    <hyperlink ref="B152" r:id="rId132"/>
+    <hyperlink ref="B153" r:id="rId133"/>
+    <hyperlink ref="B154" r:id="rId134"/>
+    <hyperlink ref="B155" r:id="rId135"/>
+    <hyperlink ref="B156" r:id="rId136"/>
+    <hyperlink ref="B157" r:id="rId137"/>
+    <hyperlink ref="B158" r:id="rId138"/>
+    <hyperlink ref="B159" r:id="rId139"/>
+    <hyperlink ref="B160" r:id="rId140"/>
+    <hyperlink ref="B161" r:id="rId141"/>
+    <hyperlink ref="B162" r:id="rId142"/>
+    <hyperlink ref="B163" r:id="rId143"/>
+    <hyperlink ref="B166" r:id="rId144"/>
+    <hyperlink ref="B167" r:id="rId145"/>
+    <hyperlink ref="B168" r:id="rId146"/>
+    <hyperlink ref="B169" r:id="rId147"/>
+    <hyperlink ref="B170" r:id="rId148"/>
+    <hyperlink ref="B171" r:id="rId149"/>
+    <hyperlink ref="B172" r:id="rId150"/>
+    <hyperlink ref="B173" r:id="rId151"/>
+    <hyperlink ref="B174" r:id="rId152"/>
+    <hyperlink ref="B177" r:id="rId153"/>
+    <hyperlink ref="B178" r:id="rId154"/>
+    <hyperlink ref="B179" r:id="rId155"/>
+    <hyperlink ref="B180" r:id="rId156"/>
+    <hyperlink ref="B181" r:id="rId157"/>
+    <hyperlink ref="B182" r:id="rId158"/>
+    <hyperlink ref="B183" r:id="rId159"/>
+    <hyperlink ref="B184" r:id="rId160"/>
+    <hyperlink ref="B185" r:id="rId161"/>
+    <hyperlink ref="B186" r:id="rId162"/>
+    <hyperlink ref="B187" r:id="rId163"/>
+    <hyperlink ref="B188" r:id="rId164"/>
+    <hyperlink ref="B189" r:id="rId165"/>
+    <hyperlink ref="B190" r:id="rId166"/>
+    <hyperlink ref="B191" r:id="rId167"/>
+    <hyperlink ref="B192" r:id="rId168"/>
+    <hyperlink ref="B193" r:id="rId169"/>
+    <hyperlink ref="B194" r:id="rId170"/>
+    <hyperlink ref="B195" r:id="rId171"/>
+    <hyperlink ref="B196" r:id="rId172"/>
+    <hyperlink ref="B197" r:id="rId173" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
+    <hyperlink ref="B198" r:id="rId174"/>
+    <hyperlink ref="B199" r:id="rId175"/>
+    <hyperlink ref="B200" r:id="rId176"/>
+    <hyperlink ref="B201" r:id="rId177"/>
+    <hyperlink ref="B202" r:id="rId178"/>
+    <hyperlink ref="B203" r:id="rId179" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
+    <hyperlink ref="B204" r:id="rId180"/>
+    <hyperlink ref="B205" r:id="rId181"/>
+    <hyperlink ref="B206" r:id="rId182"/>
+    <hyperlink ref="B207" r:id="rId183"/>
+    <hyperlink ref="B208" r:id="rId184"/>
+    <hyperlink ref="B209" r:id="rId185"/>
+    <hyperlink ref="B210" r:id="rId186"/>
+    <hyperlink ref="B211" r:id="rId187"/>
+    <hyperlink ref="B214" r:id="rId188"/>
+    <hyperlink ref="B215" r:id="rId189"/>
+    <hyperlink ref="B216" r:id="rId190"/>
+    <hyperlink ref="B217" r:id="rId191"/>
+    <hyperlink ref="B218" r:id="rId192"/>
+    <hyperlink ref="B219" r:id="rId193"/>
+    <hyperlink ref="B220" r:id="rId194"/>
+    <hyperlink ref="B221" r:id="rId195"/>
+    <hyperlink ref="B222" r:id="rId196"/>
+    <hyperlink ref="B223" r:id="rId197"/>
+    <hyperlink ref="B224" r:id="rId198"/>
+    <hyperlink ref="B225" r:id="rId199"/>
+    <hyperlink ref="B226" r:id="rId200"/>
+    <hyperlink ref="B227" r:id="rId201"/>
+    <hyperlink ref="B228" r:id="rId202"/>
+    <hyperlink ref="B229" r:id="rId203"/>
+    <hyperlink ref="B230" r:id="rId204"/>
+    <hyperlink ref="B231" r:id="rId205"/>
+    <hyperlink ref="B232" r:id="rId206"/>
+    <hyperlink ref="B233" r:id="rId207"/>
+    <hyperlink ref="B234" r:id="rId208"/>
+    <hyperlink ref="B235" r:id="rId209"/>
+    <hyperlink ref="B238" r:id="rId210"/>
+    <hyperlink ref="B239" r:id="rId211"/>
+    <hyperlink ref="B240" r:id="rId212"/>
+    <hyperlink ref="B241" r:id="rId213"/>
+    <hyperlink ref="B242" r:id="rId214"/>
+    <hyperlink ref="B243" r:id="rId215"/>
+    <hyperlink ref="B244" r:id="rId216"/>
+    <hyperlink ref="B245" r:id="rId217"/>
+    <hyperlink ref="B246" r:id="rId218"/>
+    <hyperlink ref="B247" r:id="rId219"/>
+    <hyperlink ref="B248" r:id="rId220"/>
+    <hyperlink ref="B249" r:id="rId221"/>
+    <hyperlink ref="B250" r:id="rId222"/>
+    <hyperlink ref="B251" r:id="rId223"/>
+    <hyperlink ref="B252" r:id="rId224"/>
+    <hyperlink ref="B253" r:id="rId225"/>
+    <hyperlink ref="B254" r:id="rId226"/>
+    <hyperlink ref="B255" r:id="rId227"/>
+    <hyperlink ref="B256" r:id="rId228"/>
+    <hyperlink ref="B257" r:id="rId229" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B258" r:id="rId230"/>
+    <hyperlink ref="B259" r:id="rId231"/>
+    <hyperlink ref="B260" r:id="rId232"/>
+    <hyperlink ref="B261" r:id="rId233"/>
+    <hyperlink ref="B262" r:id="rId234"/>
+    <hyperlink ref="B263" r:id="rId235"/>
+    <hyperlink ref="B264" r:id="rId236"/>
+    <hyperlink ref="B265" r:id="rId237"/>
+    <hyperlink ref="B266" r:id="rId238"/>
+    <hyperlink ref="B267" r:id="rId239"/>
+    <hyperlink ref="B268" r:id="rId240"/>
+    <hyperlink ref="B269" r:id="rId241"/>
+    <hyperlink ref="B270" r:id="rId242"/>
+    <hyperlink ref="B271" r:id="rId243"/>
+    <hyperlink ref="B272" r:id="rId244"/>
+    <hyperlink ref="B275" r:id="rId245"/>
+    <hyperlink ref="B276" r:id="rId246"/>
+    <hyperlink ref="B277" r:id="rId247"/>
+    <hyperlink ref="B278" r:id="rId248"/>
+    <hyperlink ref="B279" r:id="rId249"/>
+    <hyperlink ref="B280" r:id="rId250"/>
+    <hyperlink ref="B281" r:id="rId251"/>
+    <hyperlink ref="B282" r:id="rId252"/>
+    <hyperlink ref="B283" r:id="rId253"/>
+    <hyperlink ref="B284" r:id="rId254"/>
+    <hyperlink ref="B285" r:id="rId255"/>
+    <hyperlink ref="B286" r:id="rId256"/>
+    <hyperlink ref="B287" r:id="rId257"/>
+    <hyperlink ref="B288" r:id="rId258"/>
+    <hyperlink ref="B289" r:id="rId259"/>
+    <hyperlink ref="B290" r:id="rId260"/>
+    <hyperlink ref="B291" r:id="rId261"/>
+    <hyperlink ref="B292" r:id="rId262"/>
+    <hyperlink ref="B293" r:id="rId263"/>
+    <hyperlink ref="B296" r:id="rId264"/>
+    <hyperlink ref="B297" r:id="rId265"/>
+    <hyperlink ref="B298" r:id="rId266"/>
+    <hyperlink ref="B299" r:id="rId267"/>
+    <hyperlink ref="B300" r:id="rId268"/>
+    <hyperlink ref="B301" r:id="rId269"/>
+    <hyperlink ref="B302" r:id="rId270"/>
+    <hyperlink ref="B303" r:id="rId271"/>
+    <hyperlink ref="B304" r:id="rId272"/>
+    <hyperlink ref="B305" r:id="rId273"/>
+    <hyperlink ref="B306" r:id="rId274" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B307" r:id="rId275"/>
+    <hyperlink ref="B308" r:id="rId276"/>
+    <hyperlink ref="B309" r:id="rId277"/>
+    <hyperlink ref="B310" r:id="rId278"/>
+    <hyperlink ref="B311" r:id="rId279"/>
+    <hyperlink ref="B312" r:id="rId280"/>
+    <hyperlink ref="B313" r:id="rId281"/>
+    <hyperlink ref="B314" r:id="rId282"/>
+    <hyperlink ref="B315" r:id="rId283"/>
+    <hyperlink ref="B316" r:id="rId284"/>
+    <hyperlink ref="B317" r:id="rId285"/>
+    <hyperlink ref="B318" r:id="rId286"/>
+    <hyperlink ref="B319" r:id="rId287"/>
+    <hyperlink ref="B320" r:id="rId288"/>
+    <hyperlink ref="B321" r:id="rId289"/>
+    <hyperlink ref="B322" r:id="rId290"/>
+    <hyperlink ref="B323" r:id="rId291"/>
+    <hyperlink ref="B324" r:id="rId292"/>
+    <hyperlink ref="B325" r:id="rId293"/>
+    <hyperlink ref="B326" r:id="rId294"/>
+    <hyperlink ref="B327" r:id="rId295"/>
+    <hyperlink ref="B328" r:id="rId296"/>
+    <hyperlink ref="B329" r:id="rId297"/>
+    <hyperlink ref="B330" r:id="rId298"/>
+    <hyperlink ref="B331" r:id="rId299"/>
+    <hyperlink ref="B332" r:id="rId300"/>
+    <hyperlink ref="B333" r:id="rId301"/>
+    <hyperlink ref="B336" r:id="rId302"/>
+    <hyperlink ref="B337" r:id="rId303"/>
+    <hyperlink ref="B338" r:id="rId304"/>
+    <hyperlink ref="B339" r:id="rId305"/>
+    <hyperlink ref="B340" r:id="rId306"/>
+    <hyperlink ref="B341" r:id="rId307"/>
+    <hyperlink ref="B342" r:id="rId308"/>
+    <hyperlink ref="B343" r:id="rId309"/>
+    <hyperlink ref="B344" r:id="rId310"/>
+    <hyperlink ref="B345" r:id="rId311"/>
+    <hyperlink ref="B346" r:id="rId312"/>
+    <hyperlink ref="B347" r:id="rId313"/>
+    <hyperlink ref="B348" r:id="rId314"/>
+    <hyperlink ref="B349" r:id="rId315"/>
+    <hyperlink ref="B350" r:id="rId316"/>
+    <hyperlink ref="B351" r:id="rId317"/>
+    <hyperlink ref="B352" r:id="rId318"/>
+    <hyperlink ref="B353" r:id="rId319"/>
+    <hyperlink ref="B357" r:id="rId320"/>
+    <hyperlink ref="B358" r:id="rId321"/>
+    <hyperlink ref="B359" r:id="rId322"/>
+    <hyperlink ref="B360" r:id="rId323"/>
+    <hyperlink ref="B361" r:id="rId324"/>
+    <hyperlink ref="B362" r:id="rId325"/>
+    <hyperlink ref="B363" r:id="rId326"/>
+    <hyperlink ref="B364" r:id="rId327"/>
+    <hyperlink ref="B365" r:id="rId328"/>
+    <hyperlink ref="B366" r:id="rId329"/>
+    <hyperlink ref="B367" r:id="rId330"/>
+    <hyperlink ref="B368" r:id="rId331"/>
+    <hyperlink ref="B369" r:id="rId332"/>
+    <hyperlink ref="B370" r:id="rId333"/>
+    <hyperlink ref="B371" r:id="rId334"/>
+    <hyperlink ref="B372" r:id="rId335"/>
+    <hyperlink ref="B373" r:id="rId336"/>
+    <hyperlink ref="B374" r:id="rId337"/>
+    <hyperlink ref="B375" r:id="rId338"/>
+    <hyperlink ref="B376" r:id="rId339"/>
+    <hyperlink ref="B377" r:id="rId340"/>
+    <hyperlink ref="B378" r:id="rId341"/>
+    <hyperlink ref="B379" r:id="rId342" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B380" r:id="rId343"/>
+    <hyperlink ref="B381" r:id="rId344"/>
+    <hyperlink ref="B382" r:id="rId345"/>
+    <hyperlink ref="B383" r:id="rId346"/>
+    <hyperlink ref="B384" r:id="rId347"/>
+    <hyperlink ref="B385" r:id="rId348"/>
+    <hyperlink ref="B386" r:id="rId349"/>
+    <hyperlink ref="B387" r:id="rId350"/>
+    <hyperlink ref="B388" r:id="rId351"/>
+    <hyperlink ref="B389" r:id="rId352"/>
+    <hyperlink ref="B390" r:id="rId353"/>
+    <hyperlink ref="B391" r:id="rId354"/>
+    <hyperlink ref="B392" r:id="rId355"/>
+    <hyperlink ref="B393" r:id="rId356"/>
+    <hyperlink ref="B394" r:id="rId357"/>
+    <hyperlink ref="B396" r:id="rId358"/>
+    <hyperlink ref="B395" r:id="rId359"/>
+    <hyperlink ref="B397" r:id="rId360"/>
+    <hyperlink ref="B398" r:id="rId361"/>
+    <hyperlink ref="B399" r:id="rId362"/>
+    <hyperlink ref="B402" r:id="rId363"/>
+    <hyperlink ref="B403" r:id="rId364"/>
+    <hyperlink ref="B404" r:id="rId365"/>
+    <hyperlink ref="B405" r:id="rId366"/>
+    <hyperlink ref="B406" r:id="rId367"/>
+    <hyperlink ref="B407" r:id="rId368"/>
+    <hyperlink ref="B410" r:id="rId369"/>
+    <hyperlink ref="B411" r:id="rId370"/>
+    <hyperlink ref="B412" r:id="rId371"/>
+    <hyperlink ref="B413" r:id="rId372"/>
+    <hyperlink ref="B414" r:id="rId373"/>
+    <hyperlink ref="B415" r:id="rId374"/>
+    <hyperlink ref="B416" r:id="rId375"/>
+    <hyperlink ref="B417" r:id="rId376"/>
+    <hyperlink ref="B418" r:id="rId377"/>
+    <hyperlink ref="B419" r:id="rId378"/>
+    <hyperlink ref="B420" r:id="rId379"/>
+    <hyperlink ref="B421" r:id="rId380"/>
+    <hyperlink ref="B422" r:id="rId381"/>
+    <hyperlink ref="B423" r:id="rId382"/>
+    <hyperlink ref="B424" r:id="rId383"/>
+    <hyperlink ref="B425" r:id="rId384"/>
+    <hyperlink ref="B426" r:id="rId385"/>
+    <hyperlink ref="B427" r:id="rId386"/>
+    <hyperlink ref="B428" r:id="rId387"/>
+    <hyperlink ref="B429" r:id="rId388"/>
+    <hyperlink ref="B430" r:id="rId389"/>
+    <hyperlink ref="B431" r:id="rId390"/>
+    <hyperlink ref="B432" r:id="rId391"/>
+    <hyperlink ref="B433" r:id="rId392"/>
+    <hyperlink ref="B434" r:id="rId393"/>
+    <hyperlink ref="B435" r:id="rId394"/>
+    <hyperlink ref="B436" r:id="rId395"/>
+    <hyperlink ref="B437" r:id="rId396"/>
+    <hyperlink ref="B438" r:id="rId397"/>
+    <hyperlink ref="B439" r:id="rId398"/>
+    <hyperlink ref="B440" r:id="rId399"/>
+    <hyperlink ref="B441" r:id="rId400"/>
+    <hyperlink ref="B442" r:id="rId401"/>
+    <hyperlink ref="B443" r:id="rId402"/>
+    <hyperlink ref="B444" r:id="rId403"/>
+    <hyperlink ref="B445" r:id="rId404"/>
+    <hyperlink ref="B446" r:id="rId405"/>
+    <hyperlink ref="B447" r:id="rId406"/>
+    <hyperlink ref="B448" r:id="rId407"/>
+    <hyperlink ref="B449" r:id="rId408"/>
+    <hyperlink ref="B451" r:id="rId409"/>
+    <hyperlink ref="B450" r:id="rId410"/>
+    <hyperlink ref="B452" r:id="rId411"/>
+    <hyperlink ref="B453" r:id="rId412"/>
+    <hyperlink ref="B454" r:id="rId413"/>
+    <hyperlink ref="B455" r:id="rId414"/>
+    <hyperlink ref="B456" r:id="rId415"/>
+    <hyperlink ref="B457" r:id="rId416"/>
+    <hyperlink ref="B458" r:id="rId417"/>
+    <hyperlink ref="B459" r:id="rId418"/>
+    <hyperlink ref="B460" r:id="rId419"/>
+    <hyperlink ref="B461" r:id="rId420"/>
+    <hyperlink ref="B462" r:id="rId421"/>
+    <hyperlink ref="B469" r:id="rId422"/>
+    <hyperlink ref="B468" r:id="rId423"/>
+    <hyperlink ref="B467" r:id="rId424"/>
+    <hyperlink ref="B466" r:id="rId425"/>
+    <hyperlink ref="B465" r:id="rId426"/>
+    <hyperlink ref="B464" r:id="rId427"/>
+    <hyperlink ref="B463" r:id="rId428"/>
+    <hyperlink ref="B472" r:id="rId429"/>
+    <hyperlink ref="B473" r:id="rId430"/>
+    <hyperlink ref="B474" r:id="rId431"/>
+    <hyperlink ref="B475" r:id="rId432"/>
+    <hyperlink ref="B476" r:id="rId433"/>
+    <hyperlink ref="B477" r:id="rId434"/>
+    <hyperlink ref="B478" r:id="rId435"/>
+    <hyperlink ref="B481" r:id="rId436"/>
+    <hyperlink ref="B479" r:id="rId437"/>
+    <hyperlink ref="B480" r:id="rId438" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B356" r:id="rId439"/>
+    <hyperlink ref="B2" r:id="rId440"/>
+    <hyperlink ref="B16" r:id="rId441"/>
+    <hyperlink ref="B15" r:id="rId442"/>
+    <hyperlink ref="B14" r:id="rId443"/>
+    <hyperlink ref="B13" r:id="rId444"/>
+    <hyperlink ref="B26" r:id="rId445"/>
+    <hyperlink ref="B101" r:id="rId446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId447"/>

</xml_diff>

<commit_message>
first set completed - some issue in one topic
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1980,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+    <sheetView tabSelected="1" topLeftCell="A284" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C238" sqref="C238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3827,8 +3828,8 @@
       <c r="B177" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C177" s="4" t="s">
-        <v>3</v>
+      <c r="C177" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -4222,8 +4223,8 @@
       <c r="B214" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="C214" s="4" t="s">
-        <v>3</v>
+      <c r="C214" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="21">
@@ -4472,8 +4473,8 @@
       <c r="B238" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C238" s="4" t="s">
-        <v>3</v>
+      <c r="C238" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="21">

</xml_diff>

<commit_message>
third set done - head for couple fourth set
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="497">
   <si>
     <t>Topic:</t>
   </si>
@@ -1509,17 +1510,20 @@
     <t>not understood</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
     <t>DP Youtube- Aditya Verma</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1601,8 +1605,16 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1621,6 +1633,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1635,7 +1653,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1670,6 +1688,9 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1987,8 +2008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E541"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F157" sqref="F157"/>
+    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C411" sqref="C411:C412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2515,8 +2536,8 @@
       <c r="B51" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>3</v>
+      <c r="C51" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="21">
@@ -2575,8 +2596,8 @@
       <c r="B58" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>3</v>
+      <c r="C58" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="21">
@@ -3056,8 +3077,8 @@
       <c r="B103" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="4" t="s">
-        <v>3</v>
+      <c r="C103" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="21">
@@ -3456,8 +3477,8 @@
       <c r="B141" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C141" s="4" t="s">
-        <v>3</v>
+      <c r="C141" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21">
@@ -3845,8 +3866,8 @@
       <c r="B178" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C178" s="4" t="s">
-        <v>3</v>
+      <c r="C178" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">
@@ -3856,8 +3877,8 @@
       <c r="B179" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C179" s="4" t="s">
-        <v>3</v>
+      <c r="C179" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">
@@ -4240,8 +4261,8 @@
       <c r="B215" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C215" s="4" t="s">
-        <v>3</v>
+      <c r="C215" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="21">
@@ -4251,8 +4272,8 @@
       <c r="B216" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C216" s="4" t="s">
-        <v>3</v>
+      <c r="C216" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="21">
@@ -4490,8 +4511,8 @@
       <c r="B239" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C239" s="4" t="s">
-        <v>3</v>
+      <c r="C239" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="21">
@@ -4501,8 +4522,8 @@
       <c r="B240" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C240" s="4" t="s">
-        <v>3</v>
+      <c r="C240" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="241" spans="1:3" ht="21">
@@ -4857,37 +4878,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:3" ht="21">
+    <row r="273" spans="1:4" ht="21">
       <c r="B273" s="7"/>
       <c r="C273" s="4"/>
     </row>
-    <row r="274" spans="1:3" ht="21">
+    <row r="274" spans="1:4" ht="21">
       <c r="B274" s="7"/>
       <c r="C274" s="4"/>
     </row>
-    <row r="275" spans="1:3" ht="21">
+    <row r="275" spans="1:4" ht="21">
       <c r="A275" s="5" t="s">
         <v>264</v>
       </c>
       <c r="B275" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="C275" s="4" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" ht="21">
+      <c r="C275" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="D275" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" ht="21">
       <c r="A276" s="5" t="s">
         <v>264</v>
       </c>
       <c r="B276" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C276" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" ht="21">
+      <c r="C276" s="12" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" ht="21">
       <c r="A277" s="5" t="s">
         <v>264</v>
       </c>
@@ -4898,7 +4922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="278" spans="1:3" ht="21">
+    <row r="278" spans="1:4" ht="21">
       <c r="A278" s="5" t="s">
         <v>264</v>
       </c>
@@ -4909,7 +4933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="21">
+    <row r="279" spans="1:4" ht="21">
       <c r="A279" s="5" t="s">
         <v>264</v>
       </c>
@@ -4920,7 +4944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="280" spans="1:3" ht="21">
+    <row r="280" spans="1:4" ht="21">
       <c r="A280" s="5" t="s">
         <v>264</v>
       </c>
@@ -4931,7 +4955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="1:3" ht="21">
+    <row r="281" spans="1:4" ht="21">
       <c r="A281" s="5" t="s">
         <v>264</v>
       </c>
@@ -4942,7 +4966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="282" spans="1:3" ht="21">
+    <row r="282" spans="1:4" ht="21">
       <c r="A282" s="5" t="s">
         <v>264</v>
       </c>
@@ -4953,7 +4977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="21">
+    <row r="283" spans="1:4" ht="21">
       <c r="A283" s="5" t="s">
         <v>264</v>
       </c>
@@ -4964,7 +4988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="284" spans="1:3" ht="21">
+    <row r="284" spans="1:4" ht="21">
       <c r="A284" s="5" t="s">
         <v>264</v>
       </c>
@@ -4975,7 +4999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="285" spans="1:3" ht="21">
+    <row r="285" spans="1:4" ht="21">
       <c r="A285" s="5" t="s">
         <v>264</v>
       </c>
@@ -4986,7 +5010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="286" spans="1:3" ht="21">
+    <row r="286" spans="1:4" ht="21">
       <c r="A286" s="5" t="s">
         <v>264</v>
       </c>
@@ -4997,7 +5021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:3" ht="21">
+    <row r="287" spans="1:4" ht="21">
       <c r="A287" s="5" t="s">
         <v>264</v>
       </c>
@@ -5008,7 +5032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="288" spans="1:3" ht="21">
+    <row r="288" spans="1:4" ht="21">
       <c r="A288" s="5" t="s">
         <v>264</v>
       </c>
@@ -5100,8 +5124,8 @@
       <c r="B297" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="C297" s="4" t="s">
-        <v>3</v>
+      <c r="C297" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="21">
@@ -5111,8 +5135,8 @@
       <c r="B298" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="C298" s="4" t="s">
-        <v>3</v>
+      <c r="C298" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="21">
@@ -5526,8 +5550,8 @@
       <c r="B337" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="C337" s="4" t="s">
-        <v>3</v>
+      <c r="C337" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="21">
@@ -5537,8 +5561,8 @@
       <c r="B338" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="C338" s="4" t="s">
-        <v>3</v>
+      <c r="C338" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="21">
@@ -5732,8 +5756,8 @@
       <c r="B357" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="C357" s="4" t="s">
-        <v>3</v>
+      <c r="C357" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="21">
@@ -5743,8 +5767,8 @@
       <c r="B358" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="C358" s="4" t="s">
-        <v>3</v>
+      <c r="C358" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="21">
@@ -6224,8 +6248,8 @@
       <c r="B403" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="C403" s="4" t="s">
-        <v>3</v>
+      <c r="C403" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="21">
@@ -6235,8 +6259,8 @@
       <c r="B404" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="C404" s="4" t="s">
-        <v>3</v>
+      <c r="C404" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="405" spans="1:3" ht="21">
@@ -6298,8 +6322,8 @@
       <c r="B411" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="C411" s="4" t="s">
-        <v>3</v>
+      <c r="C411" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="21">
@@ -6309,8 +6333,8 @@
       <c r="B412" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="C412" s="4" t="s">
-        <v>3</v>
+      <c r="C412" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="21">
@@ -6967,8 +6991,8 @@
       <c r="B473" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="C473" s="4" t="s">
-        <v>3</v>
+      <c r="C473" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="474" spans="1:3" ht="21">
@@ -7061,10 +7085,13 @@
     </row>
     <row r="492" spans="1:3">
       <c r="A492" s="15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B492" s="15">
         <v>1</v>
+      </c>
+      <c r="C492" s="16" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="493" spans="1:3">
@@ -7072,17 +7099,26 @@
       <c r="B493" s="15">
         <v>2</v>
       </c>
+      <c r="C493" s="16" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="494" spans="1:3">
       <c r="A494" s="15"/>
       <c r="B494" s="15">
         <v>3</v>
+      </c>
+      <c r="C494" s="16" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="495" spans="1:3">
       <c r="A495" s="15"/>
       <c r="B495" s="15">
         <v>4</v>
+      </c>
+      <c r="C495" s="16" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="496" spans="1:3">

</xml_diff>

<commit_message>
just checking after long time
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="496">
   <si>
     <t>Topic:</t>
   </si>
@@ -1418,9 +1418,6 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
-  </si>
-  <si>
-    <t>Todays Mark</t>
   </si>
   <si>
     <t>YES</t>
@@ -2008,8 +2005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E541"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C411" sqref="C411:C412"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2051,7 +2048,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">
@@ -2062,7 +2059,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">
@@ -2073,7 +2070,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
@@ -2084,7 +2081,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
@@ -2095,7 +2092,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">
@@ -2106,7 +2103,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">
@@ -2117,7 +2114,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
@@ -2128,7 +2125,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
@@ -2139,7 +2136,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21">
@@ -2150,7 +2147,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21">
@@ -2161,7 +2158,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
@@ -2172,7 +2169,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
@@ -2183,7 +2180,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -2194,7 +2191,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">
@@ -2205,7 +2202,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21">
@@ -2216,7 +2213,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21">
@@ -2227,7 +2224,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
@@ -2238,7 +2235,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21">
@@ -2249,7 +2246,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21">
@@ -2260,7 +2257,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21">
@@ -2271,7 +2268,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21">
@@ -2282,7 +2279,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21">
@@ -2293,7 +2290,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21">
@@ -2304,7 +2301,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21">
@@ -2315,7 +2312,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21">
@@ -2326,7 +2323,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21">
@@ -2337,7 +2334,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="21">
@@ -2348,7 +2345,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="21">
@@ -2359,7 +2356,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21">
@@ -2370,7 +2367,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="21">
@@ -2381,7 +2378,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21">
@@ -2392,7 +2389,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="21">
@@ -2403,7 +2400,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="21">
@@ -2414,7 +2411,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21">
@@ -2425,7 +2422,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="21">
@@ -2436,7 +2433,7 @@
         <v>40</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21">
@@ -2460,7 +2457,7 @@
         <v>42</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">
@@ -2471,7 +2468,7 @@
         <v>43</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="21">
@@ -2482,7 +2479,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="21">
@@ -2493,7 +2490,7 @@
         <v>45</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="21">
@@ -2504,7 +2501,7 @@
         <v>46</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="21">
@@ -2515,7 +2512,7 @@
         <v>47</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="21">
@@ -2526,7 +2523,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="21">
@@ -2537,7 +2534,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="21">
@@ -2575,7 +2572,7 @@
         <v>53</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="21">
@@ -2586,7 +2583,7 @@
         <v>54</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="21">
@@ -2597,7 +2594,7 @@
         <v>55</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="21">
@@ -2607,7 +2604,7 @@
       <c r="B59" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="12" t="s">
         <v>464</v>
       </c>
     </row>
@@ -2618,8 +2615,8 @@
       <c r="B60" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>3</v>
+      <c r="C60" s="12" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="21">
@@ -2629,8 +2626,8 @@
       <c r="B61" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>3</v>
+      <c r="C61" s="12" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="21">
@@ -2666,7 +2663,7 @@
         <v>3</v>
       </c>
       <c r="E64" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">
@@ -3056,7 +3053,7 @@
         <v>97</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="21">
@@ -3067,7 +3064,7 @@
         <v>98</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="21">
@@ -3078,7 +3075,7 @@
         <v>99</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="21">
@@ -3088,8 +3085,8 @@
       <c r="B104" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C104" s="4" t="s">
-        <v>3</v>
+      <c r="C104" s="12" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="21">
@@ -3099,8 +3096,8 @@
       <c r="B105" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C105" s="4" t="s">
-        <v>3</v>
+      <c r="C105" s="12" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="21">
@@ -3110,8 +3107,8 @@
       <c r="B106" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="4" t="s">
-        <v>3</v>
+      <c r="C106" s="12" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="21">
@@ -3456,7 +3453,7 @@
         <v>134</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21">
@@ -3467,7 +3464,7 @@
         <v>135</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="21">
@@ -3478,7 +3475,7 @@
         <v>136</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21">
@@ -3488,8 +3485,8 @@
       <c r="B142" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C142" s="4" t="s">
-        <v>3</v>
+      <c r="C142" s="12" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21">
@@ -3499,8 +3496,8 @@
       <c r="B143" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C143" s="4" t="s">
-        <v>3</v>
+      <c r="C143" s="12" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="21">
@@ -3510,8 +3507,8 @@
       <c r="B144" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C144" s="4" t="s">
-        <v>3</v>
+      <c r="C144" s="12" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21">
@@ -3856,7 +3853,7 @@
         <v>171</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -3867,7 +3864,7 @@
         <v>172</v>
       </c>
       <c r="C178" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">
@@ -3878,7 +3875,7 @@
         <v>173</v>
       </c>
       <c r="C179" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">
@@ -4251,7 +4248,7 @@
         <v>207</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="21">
@@ -4262,7 +4259,7 @@
         <v>208</v>
       </c>
       <c r="C215" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="21">
@@ -4273,7 +4270,7 @@
         <v>209</v>
       </c>
       <c r="C216" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="21">
@@ -4501,7 +4498,7 @@
         <v>230</v>
       </c>
       <c r="C238" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="21">
@@ -4512,7 +4509,7 @@
         <v>231</v>
       </c>
       <c r="C239" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="21">
@@ -4523,7 +4520,7 @@
         <v>232</v>
       </c>
       <c r="C240" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="241" spans="1:3" ht="21">
@@ -4894,10 +4891,10 @@
         <v>265</v>
       </c>
       <c r="C275" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D275" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="21">
@@ -4908,7 +4905,7 @@
         <v>266</v>
       </c>
       <c r="C276" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="21">
@@ -4918,8 +4915,8 @@
       <c r="B277" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="C277" s="4" t="s">
-        <v>3</v>
+      <c r="C277" s="12" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="21">
@@ -5114,7 +5111,7 @@
         <v>285</v>
       </c>
       <c r="C296" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="21">
@@ -5125,7 +5122,7 @@
         <v>286</v>
       </c>
       <c r="C297" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="21">
@@ -5136,7 +5133,7 @@
         <v>287</v>
       </c>
       <c r="C298" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="21">
@@ -5540,7 +5537,7 @@
         <v>324</v>
       </c>
       <c r="C336" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="21">
@@ -5551,7 +5548,7 @@
         <v>325</v>
       </c>
       <c r="C337" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="21">
@@ -5562,7 +5559,7 @@
         <v>326</v>
       </c>
       <c r="C338" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="21">
@@ -5746,7 +5743,7 @@
         <v>343</v>
       </c>
       <c r="C356" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="21">
@@ -5757,7 +5754,7 @@
         <v>344</v>
       </c>
       <c r="C357" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="21">
@@ -5768,7 +5765,7 @@
         <v>345</v>
       </c>
       <c r="C358" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="21">
@@ -6238,7 +6235,7 @@
         <v>387</v>
       </c>
       <c r="C402" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="403" spans="1:3" ht="21">
@@ -6249,7 +6246,7 @@
         <v>388</v>
       </c>
       <c r="C403" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="21">
@@ -6260,7 +6257,7 @@
         <v>389</v>
       </c>
       <c r="C404" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="405" spans="1:3" ht="21">
@@ -6312,7 +6309,7 @@
         <v>393</v>
       </c>
       <c r="C410" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="21">
@@ -6323,7 +6320,7 @@
         <v>394</v>
       </c>
       <c r="C411" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="21">
@@ -6334,7 +6331,7 @@
         <v>395</v>
       </c>
       <c r="C412" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="21">
@@ -6981,7 +6978,7 @@
         <v>453</v>
       </c>
       <c r="C472" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="473" spans="1:3" ht="21">
@@ -6992,7 +6989,7 @@
         <v>454</v>
       </c>
       <c r="C473" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="474" spans="1:3" ht="21">
@@ -7002,8 +6999,8 @@
       <c r="B474" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="C474" s="4" t="s">
-        <v>3</v>
+      <c r="C474" s="12" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="475" spans="1:3" ht="21">
@@ -7083,15 +7080,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="485" spans="1:3">
+      <c r="C485">
+        <f ca="1">COUNTIF(C6:C500, "YES")</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="492" spans="1:3">
       <c r="A492" s="15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B492" s="15">
         <v>1</v>
       </c>
       <c r="C492" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="493" spans="1:3">
@@ -7100,7 +7103,7 @@
         <v>2</v>
       </c>
       <c r="C493" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="494" spans="1:3">
@@ -7109,7 +7112,7 @@
         <v>3</v>
       </c>
       <c r="C494" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="495" spans="1:3">
@@ -7118,7 +7121,7 @@
         <v>4</v>
       </c>
       <c r="C495" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="496" spans="1:3">
@@ -7863,7 +7866,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="13" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -7894,10 +7897,10 @@
     </row>
     <row r="7" spans="1:12">
       <c r="C7" t="s">
+        <v>468</v>
+      </c>
+      <c r="D7" t="s">
         <v>469</v>
-      </c>
-      <c r="D7" t="s">
-        <v>470</v>
       </c>
       <c r="E7">
         <v>-1</v>
@@ -7926,10 +7929,10 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -7940,10 +7943,10 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
+        <v>470</v>
+      </c>
+      <c r="B9" t="s">
         <v>471</v>
-      </c>
-      <c r="B9" t="s">
-        <v>472</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -7954,10 +7957,10 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -7992,10 +7995,10 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -8006,10 +8009,10 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B12" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -8020,10 +8023,10 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B13" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
@@ -8058,10 +8061,10 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
+        <v>477</v>
+      </c>
+      <c r="B14" t="s">
         <v>478</v>
-      </c>
-      <c r="B14" t="s">
-        <v>479</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -8072,12 +8075,12 @@
     </row>
     <row r="15" spans="1:12">
       <c r="B15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="14" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -8102,16 +8105,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>481</v>
+      </c>
+      <c r="B32" t="s">
         <v>482</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>483</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>484</v>
-      </c>
-      <c r="D32" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -8122,7 +8125,7 @@
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -8132,7 +8135,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -8141,7 +8144,7 @@
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -8151,7 +8154,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -8160,12 +8163,12 @@
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="D39" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -8175,7 +8178,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -8184,12 +8187,12 @@
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="D42" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="43" spans="1:4">

</xml_diff>